<commit_message>
BOM for Bluetooth Module
</commit_message>
<xml_diff>
--- a/Steering/Hardware/BOM/Steering_Controller_BOM_1R0.xlsx
+++ b/Steering/Hardware/BOM/Steering_Controller_BOM_1R0.xlsx
@@ -1,32 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git\2020-srw-rc-car\Steering\Hardware\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\files.auckland.ac.nz\myhome\Desktop\Electeng\2020-srw-rc-car\Steering\Hardware\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47C6092A-1495-4423-9FAB-884ECDC94282}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E868C7-A5BB-4A80-A4AA-08B89FE2B689}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39615" yWindow="4515" windowWidth="23835" windowHeight="11040" xr2:uid="{4895F57E-8DCF-4A6C-9607-D9B5352DA2F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -104,9 +96,6 @@
     <t>ATmega328PB SMD</t>
   </si>
   <si>
-    <t>1uF Capacitor</t>
-  </si>
-  <si>
     <t>Samsung Electro-Mechanics CAP CER 1UF 50V X5R 1206</t>
   </si>
   <si>
@@ -114,6 +103,9 @@
   </si>
   <si>
     <t>Steering Controller</t>
+  </si>
+  <si>
+    <t>4.7uF Capacitor</t>
   </si>
 </sst>
 </file>
@@ -121,7 +113,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -257,15 +249,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyBorder="1"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -587,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F14A6EB3-AA55-40DD-86B5-47847CF9DC22}">
   <dimension ref="B2:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -603,7 +595,7 @@
   <sheetData>
     <row r="2" spans="2:7" ht="34.5" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="36.75" customHeight="1">
@@ -651,10 +643,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -663,7 +655,7 @@
         <v>0.46</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:7">

</xml_diff>